<commit_message>
Update de textos webinars y fotos
</commit_message>
<xml_diff>
--- a/docs/roadmap/roadmap_lobra_v1.0.xlsx
+++ b/docs/roadmap/roadmap_lobra_v1.0.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://erpforentrepreneur-my.sharepoint.com/personal/rhuerta_myowngmail_com/Documents/Huerta Consulting/Lobra/Desarrollo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://erpforentrepreneur-my.sharepoint.com/personal/rhuerta_myowngmail_com/Documents/Huerta Consulting/Next JS/huerta-web/docs/roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F6CD7BE-E7F2-458D-91C6-2D7718D456C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{6F6CD7BE-E7F2-458D-91C6-2D7718D456C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE0C7ADF-2F1A-4D1C-BE59-F096910721BE}"/>
   <bookViews>
-    <workbookView xWindow="41025" yWindow="2040" windowWidth="28710" windowHeight="16860" xr2:uid="{91E9A9D3-1C4C-43B1-A51B-7CA43DDB5C06}"/>
+    <workbookView xWindow="32010" yWindow="390" windowWidth="39300" windowHeight="19380" activeTab="1" xr2:uid="{91E9A9D3-1C4C-43B1-A51B-7CA43DDB5C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$33</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="167">
   <si>
     <t>#</t>
   </si>
@@ -465,6 +466,81 @@
   </si>
   <si>
     <t>Fase 5</t>
+  </si>
+  <si>
+    <t>Mejora</t>
+  </si>
+  <si>
+    <t>Impacto(ventas)</t>
+  </si>
+  <si>
+    <t>Esfuerzo(técnico)</t>
+  </si>
+  <si>
+    <t>Urgencia</t>
+  </si>
+  <si>
+    <t>Prioridad sugerida</t>
+  </si>
+  <si>
+    <t>Mejorar descripción y estructura de clases individuales</t>
+  </si>
+  <si>
+    <t>1️⃣ inmediata</t>
+  </si>
+  <si>
+    <t>Página dedicada de venta de módulos</t>
+  </si>
+  <si>
+    <t>2️⃣ muy alta</t>
+  </si>
+  <si>
+    <t>Upsell en correo de confirmación</t>
+  </si>
+  <si>
+    <t>3️⃣ alta</t>
+  </si>
+  <si>
+    <t>Opción de asesoría personalizada desde páginas de webinars</t>
+  </si>
+  <si>
+    <t>4️⃣ alta</t>
+  </si>
+  <si>
+    <t>En prelobby, enlace a asesoría 1-a-1</t>
+  </si>
+  <si>
+    <t>5️⃣ media</t>
+  </si>
+  <si>
+    <t>Página de venta de uno-a-uno</t>
+  </si>
+  <si>
+    <t>6️⃣ media</t>
+  </si>
+  <si>
+    <t>Duraciones 30/60/120 min en asesorías</t>
+  </si>
+  <si>
+    <t>7️⃣ media-baja</t>
+  </si>
+  <si>
+    <t>Servicios adicionales (personalizar/configurar plantillas Excel)</t>
+  </si>
+  <si>
+    <t>8️⃣ media-baja</t>
+  </si>
+  <si>
+    <t>Selector de fechas en clases</t>
+  </si>
+  <si>
+    <t>9️⃣ baja</t>
+  </si>
+  <si>
+    <t>Destacar próximo módulo en home</t>
+  </si>
+  <si>
+    <t>🔟 baja</t>
   </si>
 </sst>
 </file>
@@ -841,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A66D3C-FB69-43A4-A164-A846238FB85E}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1014,7 +1090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1164,7 +1240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2590,4 +2666,247 @@
   <autoFilter ref="A1:O33" xr:uid="{30A66D3C-FB69-43A4-A164-A846238FB85E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EC237A-0C20-4106-ACE7-75C0AA543A6E}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update link zoom planeacion
</commit_message>
<xml_diff>
--- a/docs/roadmap/roadmap_lobra_v1.0.xlsx
+++ b/docs/roadmap/roadmap_lobra_v1.0.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://erpforentrepreneur-my.sharepoint.com/personal/rhuerta_myowngmail_com/Documents/Huerta Consulting/Next JS/huerta-web/docs/roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{6F6CD7BE-E7F2-458D-91C6-2D7718D456C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE0C7ADF-2F1A-4D1C-BE59-F096910721BE}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{6F6CD7BE-E7F2-458D-91C6-2D7718D456C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB84C233-E9FD-EC43-BF19-592886EF445F}"/>
   <bookViews>
-    <workbookView xWindow="32010" yWindow="390" windowWidth="39300" windowHeight="19380" activeTab="1" xr2:uid="{91E9A9D3-1C4C-43B1-A51B-7CA43DDB5C06}"/>
+    <workbookView xWindow="19580" yWindow="3300" windowWidth="33860" windowHeight="18960" activeTab="1" xr2:uid="{91E9A9D3-1C4C-43B1-A51B-7CA43DDB5C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$33</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="309">
   <si>
     <t>#</t>
   </si>
@@ -541,6 +542,432 @@
   </si>
   <si>
     <t>🔟 baja</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Compl</t>
+  </si>
+  <si>
+    <t>Impacto</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>Dependencia</t>
+  </si>
+  <si>
+    <t>Condición</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>Upsell en mail post-compra</t>
+  </si>
+  <si>
+    <t>Subir ticket inmediato</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>baja</t>
+  </si>
+  <si>
+    <t>muy alta</t>
+  </si>
+  <si>
+    <t>muy alto</t>
+  </si>
+  <si>
+    <t>intención máxima</t>
+  </si>
+  <si>
+    <t>mail base</t>
+  </si>
+  <si>
+    <t>ninguna</t>
+  </si>
+  <si>
+    <t>Upsell en mail de confirmación</t>
+  </si>
+  <si>
+    <t>Venta secundaria instantánea</t>
+  </si>
+  <si>
+    <t>alta</t>
+  </si>
+  <si>
+    <t>refuerzo</t>
+  </si>
+  <si>
+    <t>checkout</t>
+  </si>
+  <si>
+    <t>Página de gracias F1</t>
+  </si>
+  <si>
+    <t>Reducir fricción y abrir upsell</t>
+  </si>
+  <si>
+    <t>primer punto crítico</t>
+  </si>
+  <si>
+    <t>Order bump en checkout</t>
+  </si>
+  <si>
+    <t>Aumentar ticket sin fricción</t>
+  </si>
+  <si>
+    <t>clic pre-pago</t>
+  </si>
+  <si>
+    <t>Precio ancla/ahorro</t>
+  </si>
+  <si>
+    <t>Cambiar percepción</t>
+  </si>
+  <si>
+    <t>decisión rápida</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>Garantía explícita</t>
+  </si>
+  <si>
+    <t>Reducir objeciones</t>
+  </si>
+  <si>
+    <t>muy baja</t>
+  </si>
+  <si>
+    <t>extremo</t>
+  </si>
+  <si>
+    <t>texto</t>
+  </si>
+  <si>
+    <t>Tiers Básico/Pro/Pro+1a1</t>
+  </si>
+  <si>
+    <t>Mover al ticket medio/alto</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>alto</t>
+  </si>
+  <si>
+    <t>empaquetado</t>
+  </si>
+  <si>
+    <t>pricing</t>
+  </si>
+  <si>
+    <t>Bundles avanzados</t>
+  </si>
+  <si>
+    <t>Ticket alto</t>
+  </si>
+  <si>
+    <t>combinación</t>
+  </si>
+  <si>
+    <t>SKUs</t>
+  </si>
+  <si>
+    <t>Prelobby con upsell</t>
+  </si>
+  <si>
+    <t>Capturar venta adicional</t>
+  </si>
+  <si>
+    <t>continuidad</t>
+  </si>
+  <si>
+    <t>gracias F1</t>
+  </si>
+  <si>
+    <t>Testimonios antes/después</t>
+  </si>
+  <si>
+    <t>Credibilidad rápida</t>
+  </si>
+  <si>
+    <t>prueba social</t>
+  </si>
+  <si>
+    <t>contenido</t>
+  </si>
+  <si>
+    <t>Beneficios cuantificados</t>
+  </si>
+  <si>
+    <t>Mostrar valor real</t>
+  </si>
+  <si>
+    <t>racionalización</t>
+  </si>
+  <si>
+    <t>datos</t>
+  </si>
+  <si>
+    <t>Featured home con módulos reales</t>
+  </si>
+  <si>
+    <t>Mejorar entrada al funnel</t>
+  </si>
+  <si>
+    <t>media-alta</t>
+  </si>
+  <si>
+    <t>medio</t>
+  </si>
+  <si>
+    <t>top funnel</t>
+  </si>
+  <si>
+    <t>datos módulo</t>
+  </si>
+  <si>
+    <t>Página comparativa</t>
+  </si>
+  <si>
+    <t>Clarificar decisión</t>
+  </si>
+  <si>
+    <t>reduce indecisión</t>
+  </si>
+  <si>
+    <t>precios</t>
+  </si>
+  <si>
+    <t>Página de gracias F2 (ThankyouModel)</t>
+  </si>
+  <si>
+    <t>Base común</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>evita duplicar</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>2 upsells consolidados</t>
+  </si>
+  <si>
+    <t>Página de gracias F3</t>
+  </si>
+  <si>
+    <t>Unificar correos/hub</t>
+  </si>
+  <si>
+    <t>bajo</t>
+  </si>
+  <si>
+    <t>expansión futura</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>ThankyouModel</t>
+  </si>
+  <si>
+    <t>Notificador interno Stripe</t>
+  </si>
+  <si>
+    <t>Evitar pérdidas</t>
+  </si>
+  <si>
+    <t>control crítico</t>
+  </si>
+  <si>
+    <t>webhooks</t>
+  </si>
+  <si>
+    <t>Integración Brevo</t>
+  </si>
+  <si>
+    <t>Nurturing</t>
+  </si>
+  <si>
+    <t>escalar leads</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Secuencia post-registro</t>
+  </si>
+  <si>
+    <t>Convertir frío→pago</t>
+  </si>
+  <si>
+    <t>baja-media</t>
+  </si>
+  <si>
+    <t>retargeting</t>
+  </si>
+  <si>
+    <t>Brevo</t>
+  </si>
+  <si>
+    <t>Brevo activo</t>
+  </si>
+  <si>
+    <t>GTM+GA4+Pixel</t>
+  </si>
+  <si>
+    <t>Tracking coherente</t>
+  </si>
+  <si>
+    <t>medición</t>
+  </si>
+  <si>
+    <t>SDK</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>SEO técnico</t>
+  </si>
+  <si>
+    <t>Visibilidad</t>
+  </si>
+  <si>
+    <t>largo plazo</t>
+  </si>
+  <si>
+    <t>sitio</t>
+  </si>
+  <si>
+    <t>Herramientas templates/pdf</t>
+  </si>
+  <si>
+    <t>Nuevo revenue stream</t>
+  </si>
+  <si>
+    <t>catálogo</t>
+  </si>
+  <si>
+    <t>assets</t>
+  </si>
+  <si>
+    <t>Sistema referidos/afiliados</t>
+  </si>
+  <si>
+    <t>Tráfico externo</t>
+  </si>
+  <si>
+    <t>expansión</t>
+  </si>
+  <si>
+    <t>stack fijo</t>
+  </si>
+  <si>
+    <t>sitio estable</t>
+  </si>
+  <si>
+    <t>Página 1a1 estática revisión</t>
+  </si>
+  <si>
+    <t>Solución temporal</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>muy bajo</t>
+  </si>
+  <si>
+    <t>no vende/no evita costo</t>
+  </si>
+  <si>
+    <t>cuando exista generador dinámico servicios</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Ofrecer un producto complementario en el correo que llega justo después de pagar.</t>
+  </si>
+  <si>
+    <t>Agregar una oferta adicional en el correo automático que confirma la compra.</t>
+  </si>
+  <si>
+    <t>Versión rápida mejorada de la página para reducir fricción y mostrar próximos pasos.</t>
+  </si>
+  <si>
+    <t>Pequeño add-on de bajo costo que se agrega con un check antes de pagar.</t>
+  </si>
+  <si>
+    <t>Mostrar precio original y ahorro para aumentar percepción de valor.</t>
+  </si>
+  <si>
+    <t>Mensaje de garantía contundente que elimina objeciones antes de comprar.</t>
+  </si>
+  <si>
+    <t>Tres versiones del mismo módulo con diferente nivel de valor para aumentar ticket promedio.</t>
+  </si>
+  <si>
+    <t>Paquetes combinados (módulo + plantilla + 1-a-1) para incrementar valor percibido.</t>
+  </si>
+  <si>
+    <t>Pantalla intermedia después de pagar que sugiere una oferta adicional.</t>
+  </si>
+  <si>
+    <t>Casos reales con cambios medibles para aumentar credibilidad inmediata.</t>
+  </si>
+  <si>
+    <t>Explicar el impacto financiero con números concretos para justificar la compra.</t>
+  </si>
+  <si>
+    <t>Mostrar módulos actuales en el home para dirigir tráfico a ventas reales.</t>
+  </si>
+  <si>
+    <t>Tabla que contrasta diferencias entre paquetes para facilitar decisión.</t>
+  </si>
+  <si>
+    <t>Modelo unificado que estandariza cómo se construyen las páginas de gracias.</t>
+  </si>
+  <si>
+    <t>Extensión del modelo para sincronizar páginas, correos y hubs en un solo sistema.</t>
+  </si>
+  <si>
+    <t>Alerta interna inmediata cuando hay compras o errores en eventos Stripe.</t>
+  </si>
+  <si>
+    <t>Conectar el sitio con Brevo para correos de marketing y automatizaciones.</t>
+  </si>
+  <si>
+    <t>Tres correos automáticos que convierten leads fríos en compradores.</t>
+  </si>
+  <si>
+    <t>Infraestructura de tracking para medir eventos y optimizar campañas.</t>
+  </si>
+  <si>
+    <t>Ajustes técnicos para mejorar indexación y tráfico orgánico.</t>
+  </si>
+  <si>
+    <t>Venta de plantillas y documentos descargables como productos adicionales.</t>
+  </si>
+  <si>
+    <t>Módulo para pagar comisiones por referidos y atraer nuevos clientes.</t>
+  </si>
+  <si>
+    <t>Revisar la página 1-a-1 hecha como solución rápida para eventual versión dinámica.</t>
   </si>
 </sst>
 </file>
@@ -556,12 +983,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -576,11 +1009,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,30 +1351,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A66D3C-FB69-43A4-A164-A846238FB85E}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="56.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +1424,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>23</v>
       </c>
@@ -1040,7 +1474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1090,7 +1524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1140,7 +1574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1190,7 +1624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1240,7 +1674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1290,7 +1724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>14</v>
       </c>
@@ -1340,7 +1774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>24</v>
       </c>
@@ -1390,7 +1824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1440,7 +1874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>13</v>
       </c>
@@ -1490,7 +1924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7</v>
       </c>
@@ -1540,7 +1974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1590,7 +2024,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1640,7 +2074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1690,7 +2124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -1740,7 +2174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1790,7 +2224,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1840,7 +2274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1890,7 +2324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1940,7 +2374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1990,7 +2424,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2040,7 +2474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2090,7 +2524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>25</v>
       </c>
@@ -2140,7 +2574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
@@ -2190,7 +2624,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>12</v>
       </c>
@@ -2240,7 +2674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2290,7 +2724,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2340,7 +2774,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2390,7 +2824,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2440,7 +2874,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2490,7 +2924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>21</v>
       </c>
@@ -2540,7 +2974,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>22</v>
       </c>
@@ -2590,7 +3024,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>1</v>
       </c>
@@ -2598,7 +3032,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="D38">
         <v>1</v>
       </c>
@@ -2606,7 +3040,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="D39">
         <v>2</v>
       </c>
@@ -2614,7 +3048,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="D40">
         <v>3</v>
       </c>
@@ -2622,7 +3056,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>2</v>
       </c>
@@ -2630,7 +3064,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="D43">
         <v>1</v>
       </c>
@@ -2638,7 +3072,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="D44">
         <v>2</v>
       </c>
@@ -2646,7 +3080,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="D45">
         <v>3</v>
       </c>
@@ -2654,7 +3088,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="D46">
         <v>4</v>
       </c>
@@ -2669,24 +3103,889 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0806EF7D-AC1B-4443-873F-57880793B1C9}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" t="s">
+        <v>186</v>
+      </c>
+      <c r="I3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" t="s">
+        <v>190</v>
+      </c>
+      <c r="I4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" t="s">
+        <v>193</v>
+      </c>
+      <c r="I5" t="s">
+        <v>187</v>
+      </c>
+      <c r="J5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I6" t="s">
+        <v>197</v>
+      </c>
+      <c r="J6" t="s">
+        <v>182</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H7" t="s">
+        <v>202</v>
+      </c>
+      <c r="I7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J7" t="s">
+        <v>182</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" t="s">
+        <v>206</v>
+      </c>
+      <c r="H8" t="s">
+        <v>207</v>
+      </c>
+      <c r="I8" t="s">
+        <v>208</v>
+      </c>
+      <c r="J8" t="s">
+        <v>182</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" t="s">
+        <v>211</v>
+      </c>
+      <c r="I9" t="s">
+        <v>212</v>
+      </c>
+      <c r="J9" t="s">
+        <v>182</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" t="s">
+        <v>206</v>
+      </c>
+      <c r="H10" t="s">
+        <v>215</v>
+      </c>
+      <c r="I10" t="s">
+        <v>216</v>
+      </c>
+      <c r="J10" t="s">
+        <v>182</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" t="s">
+        <v>295</v>
+      </c>
+      <c r="C11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" t="s">
+        <v>185</v>
+      </c>
+      <c r="G11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H11" t="s">
+        <v>219</v>
+      </c>
+      <c r="I11" t="s">
+        <v>220</v>
+      </c>
+      <c r="J11" t="s">
+        <v>182</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F12" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" t="s">
+        <v>201</v>
+      </c>
+      <c r="H12" t="s">
+        <v>223</v>
+      </c>
+      <c r="I12" t="s">
+        <v>224</v>
+      </c>
+      <c r="J12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>225</v>
+      </c>
+      <c r="B13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" t="s">
+        <v>227</v>
+      </c>
+      <c r="G13" t="s">
+        <v>228</v>
+      </c>
+      <c r="H13" t="s">
+        <v>229</v>
+      </c>
+      <c r="I13" t="s">
+        <v>230</v>
+      </c>
+      <c r="J13" t="s">
+        <v>182</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14" t="s">
+        <v>298</v>
+      </c>
+      <c r="C14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G14" t="s">
+        <v>206</v>
+      </c>
+      <c r="H14" t="s">
+        <v>233</v>
+      </c>
+      <c r="I14" t="s">
+        <v>234</v>
+      </c>
+      <c r="J14" t="s">
+        <v>182</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" t="s">
+        <v>299</v>
+      </c>
+      <c r="C15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" t="s">
+        <v>237</v>
+      </c>
+      <c r="E15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F15" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H15" t="s">
+        <v>238</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
+      </c>
+      <c r="J15" t="s">
+        <v>240</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>241</v>
+      </c>
+      <c r="B16" t="s">
+        <v>300</v>
+      </c>
+      <c r="C16" t="s">
+        <v>242</v>
+      </c>
+      <c r="D16" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F16" t="s">
+        <v>205</v>
+      </c>
+      <c r="G16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H16" t="s">
+        <v>244</v>
+      </c>
+      <c r="I16" t="s">
+        <v>245</v>
+      </c>
+      <c r="J16" t="s">
+        <v>246</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B17" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" t="s">
+        <v>237</v>
+      </c>
+      <c r="E17" t="s">
+        <v>205</v>
+      </c>
+      <c r="F17" t="s">
+        <v>205</v>
+      </c>
+      <c r="G17" t="s">
+        <v>228</v>
+      </c>
+      <c r="H17" t="s">
+        <v>249</v>
+      </c>
+      <c r="I17" t="s">
+        <v>250</v>
+      </c>
+      <c r="J17" t="s">
+        <v>182</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" t="s">
+        <v>302</v>
+      </c>
+      <c r="C18" t="s">
+        <v>252</v>
+      </c>
+      <c r="D18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E18" t="s">
+        <v>205</v>
+      </c>
+      <c r="F18" t="s">
+        <v>227</v>
+      </c>
+      <c r="G18" t="s">
+        <v>228</v>
+      </c>
+      <c r="H18" t="s">
+        <v>253</v>
+      </c>
+      <c r="I18" t="s">
+        <v>254</v>
+      </c>
+      <c r="J18" t="s">
+        <v>182</v>
+      </c>
+      <c r="K18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C19" t="s">
+        <v>256</v>
+      </c>
+      <c r="D19" t="s">
+        <v>237</v>
+      </c>
+      <c r="E19" t="s">
+        <v>257</v>
+      </c>
+      <c r="F19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G19" t="s">
+        <v>206</v>
+      </c>
+      <c r="H19" t="s">
+        <v>258</v>
+      </c>
+      <c r="I19" t="s">
+        <v>259</v>
+      </c>
+      <c r="J19" t="s">
+        <v>260</v>
+      </c>
+      <c r="K19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>261</v>
+      </c>
+      <c r="B20" t="s">
+        <v>304</v>
+      </c>
+      <c r="C20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D20" t="s">
+        <v>237</v>
+      </c>
+      <c r="E20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F20" t="s">
+        <v>205</v>
+      </c>
+      <c r="G20" t="s">
+        <v>228</v>
+      </c>
+      <c r="H20" t="s">
+        <v>263</v>
+      </c>
+      <c r="I20" t="s">
+        <v>264</v>
+      </c>
+      <c r="J20" t="s">
+        <v>265</v>
+      </c>
+      <c r="K20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>266</v>
+      </c>
+      <c r="B21" t="s">
+        <v>305</v>
+      </c>
+      <c r="C21" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21" t="s">
+        <v>237</v>
+      </c>
+      <c r="E21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" t="s">
+        <v>243</v>
+      </c>
+      <c r="H21" t="s">
+        <v>268</v>
+      </c>
+      <c r="I21" t="s">
+        <v>269</v>
+      </c>
+      <c r="J21" t="s">
+        <v>182</v>
+      </c>
+      <c r="K21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22" t="s">
+        <v>306</v>
+      </c>
+      <c r="C22" t="s">
+        <v>271</v>
+      </c>
+      <c r="D22" t="s">
+        <v>237</v>
+      </c>
+      <c r="E22" t="s">
+        <v>205</v>
+      </c>
+      <c r="F22" t="s">
+        <v>205</v>
+      </c>
+      <c r="G22" t="s">
+        <v>228</v>
+      </c>
+      <c r="H22" t="s">
+        <v>272</v>
+      </c>
+      <c r="I22" t="s">
+        <v>273</v>
+      </c>
+      <c r="J22" t="s">
+        <v>182</v>
+      </c>
+      <c r="K22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>274</v>
+      </c>
+      <c r="B23" t="s">
+        <v>307</v>
+      </c>
+      <c r="C23" t="s">
+        <v>275</v>
+      </c>
+      <c r="D23" t="s">
+        <v>237</v>
+      </c>
+      <c r="E23" t="s">
+        <v>227</v>
+      </c>
+      <c r="F23" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23" t="s">
+        <v>228</v>
+      </c>
+      <c r="H23" t="s">
+        <v>276</v>
+      </c>
+      <c r="I23" t="s">
+        <v>277</v>
+      </c>
+      <c r="J23" t="s">
+        <v>278</v>
+      </c>
+      <c r="K23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" t="s">
+        <v>308</v>
+      </c>
+      <c r="C24" t="s">
+        <v>280</v>
+      </c>
+      <c r="D24" t="s">
+        <v>281</v>
+      </c>
+      <c r="E24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" t="s">
+        <v>177</v>
+      </c>
+      <c r="G24" t="s">
+        <v>282</v>
+      </c>
+      <c r="H24" t="s">
+        <v>283</v>
+      </c>
+      <c r="I24" t="s">
+        <v>182</v>
+      </c>
+      <c r="J24" t="s">
+        <v>284</v>
+      </c>
+      <c r="K24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EC237A-0C20-4106-ACE7-75C0AA543A6E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2706,47 +4005,47 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>7</v>
       </c>
@@ -2766,7 +4065,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2786,7 +4085,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2806,27 +4105,27 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9</v>
       </c>
@@ -2846,7 +4145,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2866,7 +4165,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2886,7 +4185,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
landing pages / Brevo / security patch
</commit_message>
<xml_diff>
--- a/docs/roadmap/roadmap_lobra_v1.0.xlsx
+++ b/docs/roadmap/roadmap_lobra_v1.0.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://erpforentrepreneur-my.sharepoint.com/personal/rhuerta_myowngmail_com/Documents/Huerta Consulting/Next JS/huerta-web/docs/roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{6F6CD7BE-E7F2-458D-91C6-2D7718D456C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1C4DFE5-4F6C-4F64-9EA9-185D8F54AEFC}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{6F6CD7BE-E7F2-458D-91C6-2D7718D456C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0848F76F-659C-4238-B9B6-E0926FE4D434}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="13965" yWindow="1920" windowWidth="30015" windowHeight="16860" activeTab="1" xr2:uid="{91E9A9D3-1C4C-43B1-A51B-7CA43DDB5C06}"/>
+    <workbookView xWindow="29625" yWindow="1455" windowWidth="28590" windowHeight="14715" activeTab="4" xr2:uid="{91E9A9D3-1C4C-43B1-A51B-7CA43DDB5C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$33</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="485">
   <si>
     <t>#</t>
   </si>
@@ -965,6 +967,537 @@
   </si>
   <si>
     <t>Revisar versión temporal.</t>
+  </si>
+  <si>
+    <t>Upsell checkout 1a1</t>
+  </si>
+  <si>
+    <t>Agregar oferta de sesión 1a1 en checkout de módulos.</t>
+  </si>
+  <si>
+    <t>checkout Stripe</t>
+  </si>
+  <si>
+    <t>Upsell checkout clase→módulo</t>
+  </si>
+  <si>
+    <t>Convertir clase individual en módulo completo desde checkout.</t>
+  </si>
+  <si>
+    <t>Aumentar ticket en compradores de clase</t>
+  </si>
+  <si>
+    <t>usuario ya paga algo</t>
+  </si>
+  <si>
+    <t>checkout clases</t>
+  </si>
+  <si>
+    <t>solo productos clase</t>
+  </si>
+  <si>
+    <t>Tiers módulo Básico/Pro/Premium</t>
+  </si>
+  <si>
+    <t>3 niveles: Básico (clases+plantilla), Pro (herramientas extra), Premium (1a1).</t>
+  </si>
+  <si>
+    <t>Subir ticket promedio</t>
+  </si>
+  <si>
+    <t>precio ancla</t>
+  </si>
+  <si>
+    <t>pricing módulos</t>
+  </si>
+  <si>
+    <t>Upsell email confirmación módulo→1a1</t>
+  </si>
+  <si>
+    <t>Oferta de 1a1 en correo de confirmación al comprar módulo.</t>
+  </si>
+  <si>
+    <t>Venta secundaria inmediata</t>
+  </si>
+  <si>
+    <t>usuario caliente</t>
+  </si>
+  <si>
+    <t>correo transaccional</t>
+  </si>
+  <si>
+    <t>Upsell email confirmación webinar→módulo/1a1</t>
+  </si>
+  <si>
+    <t>Oferta de módulo o 1a1 tras registro de webinar.</t>
+  </si>
+  <si>
+    <t>Convertir leads tibios en ventas</t>
+  </si>
+  <si>
+    <t>intención clara</t>
+  </si>
+  <si>
+    <t>correo webinar</t>
+  </si>
+  <si>
+    <t>si existe módulo o 1a1</t>
+  </si>
+  <si>
+    <t>Destacar siguiente módulo en home</t>
+  </si>
+  <si>
+    <t>Mostrar módulo prioritario con lógica correcta.</t>
+  </si>
+  <si>
+    <t>Dirigir tráfico a oferta principal</t>
+  </si>
+  <si>
+    <t>medio-alto</t>
+  </si>
+  <si>
+    <t>entra por home</t>
+  </si>
+  <si>
+    <t>datos módulos</t>
+  </si>
+  <si>
+    <t>Banner/popup cupón entrada</t>
+  </si>
+  <si>
+    <t>Cupon X% por email al entrar (versión simple sin Brevo).</t>
+  </si>
+  <si>
+    <t>Captar leads y empujar compra inicial</t>
+  </si>
+  <si>
+    <t>rápido de implementar</t>
+  </si>
+  <si>
+    <t>form simple</t>
+  </si>
+  <si>
+    <t>futuro conectar Brevo</t>
+  </si>
+  <si>
+    <t>Múltiples fechas por clase individual</t>
+  </si>
+  <si>
+    <t>Permitir elegir entre varias fechas por clase.</t>
+  </si>
+  <si>
+    <t>Aumentar conversiones de clases sueltas</t>
+  </si>
+  <si>
+    <t>flexibilidad</t>
+  </si>
+  <si>
+    <t>agenda clases</t>
+  </si>
+  <si>
+    <t>Meta Ads (Facebook/Instagram)</t>
+  </si>
+  <si>
+    <t>Campañas de venta de módulos con pixel completo.</t>
+  </si>
+  <si>
+    <t>Generar ventas directas con tráfico frío/tibio</t>
+  </si>
+  <si>
+    <t>alto alcance</t>
+  </si>
+  <si>
+    <t>GTM+Pixel+funnels optimizados</t>
+  </si>
+  <si>
+    <t>activable tras tareas 1–7</t>
+  </si>
+  <si>
+    <t>Google Ads (Search)</t>
+  </si>
+  <si>
+    <t>Captar intención directa en búsquedas relevantes.</t>
+  </si>
+  <si>
+    <t>Ventas por demanda activa</t>
+  </si>
+  <si>
+    <t>A/B</t>
+  </si>
+  <si>
+    <t>intención explícita</t>
+  </si>
+  <si>
+    <t>landing optimizada+SEO técnico</t>
+  </si>
+  <si>
+    <t>post-optimización tiers/home</t>
+  </si>
+  <si>
+    <t>Versión rápida con próximos pasos y CTA.</t>
+  </si>
+  <si>
+    <t>Reducir fricción inmediata</t>
+  </si>
+  <si>
+    <t>Modelo unificado para thanks y upsells.</t>
+  </si>
+  <si>
+    <t>Ecosistema coherente</t>
+  </si>
+  <si>
+    <t>refactor final</t>
+  </si>
+  <si>
+    <t>Alerta en compras y errores.</t>
+  </si>
+  <si>
+    <t>Conectar listas, segmentos y envíos.</t>
+  </si>
+  <si>
+    <t>Nurturing y campañas</t>
+  </si>
+  <si>
+    <t>impulsa leads</t>
+  </si>
+  <si>
+    <t>API Brevo</t>
+  </si>
+  <si>
+    <t>3 correos automáticos para leads.</t>
+  </si>
+  <si>
+    <t>Medición y optimización</t>
+  </si>
+  <si>
+    <t>base para ads</t>
+  </si>
+  <si>
+    <t>Indexación adecuada.</t>
+  </si>
+  <si>
+    <t>Visibilidad orgánica</t>
+  </si>
+  <si>
+    <t>impacto largo plazo</t>
+  </si>
+  <si>
+    <t>Productos extra descargables.</t>
+  </si>
+  <si>
+    <t>aumenta valor Pro</t>
+  </si>
+  <si>
+    <t>Comisiones a referidos.</t>
+  </si>
+  <si>
+    <t>Tracción vía comunidad</t>
+  </si>
+  <si>
+    <t>escala orgánica</t>
+  </si>
+  <si>
+    <t>stack estable</t>
+  </si>
+  <si>
+    <t>tras más alumnos</t>
+  </si>
+  <si>
+    <t>Revisar solución temporal para futura versión dinámica.</t>
+  </si>
+  <si>
+    <t>Evitar deuda futura menor</t>
+  </si>
+  <si>
+    <t>no genera ventas</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>Tarea</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Dependencias</t>
+  </si>
+  <si>
+    <t>Fecha_límite</t>
+  </si>
+  <si>
+    <t>Esfuerzo(horas)</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>Oferta/SalesPage</t>
+  </si>
+  <si>
+    <t>Optimizar_sales_page_(testimonios,_quién_soy,_transformación)</t>
+  </si>
+  <si>
+    <t>Aumentar_conversión_en_página</t>
+  </si>
+  <si>
+    <t>Indispensable</t>
+  </si>
+  <si>
+    <t>Ninguna</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>Integrar_prueba_social_en_formato_texto</t>
+  </si>
+  <si>
+    <t>Construir_confianza</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>Integrar_prueba_social_en_formato_video</t>
+  </si>
+  <si>
+    <t>Probar_autoridad_visual</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>Unificar_detalle_de_módulos_en_la_sales_page</t>
+  </si>
+  <si>
+    <t>Claridad_y_valor</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>Agregar_bloque_de_garantía</t>
+  </si>
+  <si>
+    <t>Reducir_objeciones</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>Agregar_bloque_valor_vs_precio</t>
+  </si>
+  <si>
+    <t>Aumentar_tasa_de_compra</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>Contenido</t>
+  </si>
+  <si>
+    <t>Grabar_reel_principal_de_atracción</t>
+  </si>
+  <si>
+    <t>Generar_tráfico_frío_y_tibio</t>
+  </si>
+  <si>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>Grabar_reel_secundario_#1</t>
+  </si>
+  <si>
+    <t>Refuerzo_de_tráfico</t>
+  </si>
+  <si>
+    <t>B03</t>
+  </si>
+  <si>
+    <t>Grabar_reel_secundario_#2</t>
+  </si>
+  <si>
+    <t>B04</t>
+  </si>
+  <si>
+    <t>Grabar_mini_clase_pregrabada_(10-12_min)</t>
+  </si>
+  <si>
+    <t>Autoridad_y_nurture</t>
+  </si>
+  <si>
+    <t>B05</t>
+  </si>
+  <si>
+    <t>ClasesGratuitas</t>
+  </si>
+  <si>
+    <t>Preparar_guion_clase_gratuita_#1_(9_dic)</t>
+  </si>
+  <si>
+    <t>Funnel_de_intención</t>
+  </si>
+  <si>
+    <t>B06</t>
+  </si>
+  <si>
+    <t>Ejecutar_clase_gratuita_#1_(9_dic)</t>
+  </si>
+  <si>
+    <t>Generar_leads_tibios</t>
+  </si>
+  <si>
+    <t>B07</t>
+  </si>
+  <si>
+    <t>Preparar_guion_clase_gratuita_#2_(16_dic)</t>
+  </si>
+  <si>
+    <t>B08</t>
+  </si>
+  <si>
+    <t>Ejecutar_clase_gratuita_#2_(16_dic)</t>
+  </si>
+  <si>
+    <t>Generar_leads_calientes</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>Crear_landing_de_captura_para_clase_gratuita</t>
+  </si>
+  <si>
+    <t>Capturar_datos_previos_a_campaña</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>Configurar_formulario_con_GA4_y_Pixel_lead_event</t>
+  </si>
+  <si>
+    <t>Tracking_para_ads</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>Configurar_página_de_confirmación_registro</t>
+  </si>
+  <si>
+    <t>Microcompromiso</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>Integración_mínima_de_Brevo_(lista_y_plantilla)</t>
+  </si>
+  <si>
+    <t>Poder_enviar_correos</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>Nurture</t>
+  </si>
+  <si>
+    <t>Crear_correo_confirmación_registro</t>
+  </si>
+  <si>
+    <t>Activación_inmediata</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>Crear_correo_post_clase_gratuita_#1</t>
+  </si>
+  <si>
+    <t>Convertir_leads_tibios</t>
+  </si>
+  <si>
+    <t>D03</t>
+  </si>
+  <si>
+    <t>Crear_correo_quick_win_con_CTA</t>
+  </si>
+  <si>
+    <t>Aumentar_intención_de_compra</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>Tracking</t>
+  </si>
+  <si>
+    <t>Validar_begin_checkout</t>
+  </si>
+  <si>
+    <t>Medición_core</t>
+  </si>
+  <si>
+    <t>E02</t>
+  </si>
+  <si>
+    <t>Validar_purchase</t>
+  </si>
+  <si>
+    <t>E03</t>
+  </si>
+  <si>
+    <t>Implementar_add_payment_info</t>
+  </si>
+  <si>
+    <t>Optimizar_anuncios</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>Estrategia</t>
+  </si>
+  <si>
+    <t>Definir_transformación_final_del_módulo</t>
+  </si>
+  <si>
+    <t>Mensaje_central</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>Definir_CTA_único_para_todo_el_embudo</t>
+  </si>
+  <si>
+    <t>Consistencia_de_mensajes</t>
+  </si>
+  <si>
+    <t>F03</t>
+  </si>
+  <si>
+    <t>Cerrar_narrativa_del_pitch_para_las_clases</t>
+  </si>
+  <si>
+    <t>Mejorar_conversión</t>
   </si>
 </sst>
 </file>
@@ -980,7 +1513,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -990,6 +1523,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,12 +1545,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1348,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A66D3C-FB69-43A4-A164-A846238FB85E}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,46 +2016,46 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>1.67</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>8</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="3" t="s">
         <v>82</v>
       </c>
       <c r="O3" t="s">
@@ -1522,46 +2066,46 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3">
         <v>5</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>1.67</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>6</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="3" t="s">
         <v>82</v>
       </c>
       <c r="O4" t="s">
@@ -1722,46 +2266,46 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
         <v>4</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>1.33</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <v>6</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="3" t="s">
         <v>88</v>
       </c>
       <c r="O8" t="s">
@@ -3103,13 +3647,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0806EF7D-AC1B-4443-873F-57880793B1C9}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:B24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
@@ -3972,7 +4516,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4208,4 +4752,1727 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FF87B5-0DBC-4E4D-974A-50BC9787346E}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" t="s">
+        <v>310</v>
+      </c>
+      <c r="J2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J3" t="s">
+        <v>316</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H4" t="s">
+        <v>320</v>
+      </c>
+      <c r="I4" t="s">
+        <v>321</v>
+      </c>
+      <c r="J4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" t="s">
+        <v>324</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" t="s">
+        <v>325</v>
+      </c>
+      <c r="I5" t="s">
+        <v>326</v>
+      </c>
+      <c r="J5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" t="s">
+        <v>255</v>
+      </c>
+      <c r="F6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H6" t="s">
+        <v>330</v>
+      </c>
+      <c r="I6" t="s">
+        <v>331</v>
+      </c>
+      <c r="J6" t="s">
+        <v>332</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>333</v>
+      </c>
+      <c r="B7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G7" t="s">
+        <v>336</v>
+      </c>
+      <c r="H7" t="s">
+        <v>337</v>
+      </c>
+      <c r="I7" t="s">
+        <v>338</v>
+      </c>
+      <c r="J7" t="s">
+        <v>182</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C8" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G8" t="s">
+        <v>336</v>
+      </c>
+      <c r="H8" t="s">
+        <v>342</v>
+      </c>
+      <c r="I8" t="s">
+        <v>343</v>
+      </c>
+      <c r="J8" t="s">
+        <v>344</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" t="s">
+        <v>204</v>
+      </c>
+      <c r="F9" t="s">
+        <v>204</v>
+      </c>
+      <c r="G9" t="s">
+        <v>227</v>
+      </c>
+      <c r="H9" t="s">
+        <v>348</v>
+      </c>
+      <c r="I9" t="s">
+        <v>349</v>
+      </c>
+      <c r="J9" t="s">
+        <v>182</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>350</v>
+      </c>
+      <c r="B10" t="s">
+        <v>351</v>
+      </c>
+      <c r="C10" t="s">
+        <v>352</v>
+      </c>
+      <c r="D10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F10" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" t="s">
+        <v>205</v>
+      </c>
+      <c r="H10" t="s">
+        <v>353</v>
+      </c>
+      <c r="I10" t="s">
+        <v>354</v>
+      </c>
+      <c r="J10" t="s">
+        <v>355</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B11" t="s">
+        <v>357</v>
+      </c>
+      <c r="C11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D11" t="s">
+        <v>359</v>
+      </c>
+      <c r="E11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F11" t="s">
+        <v>226</v>
+      </c>
+      <c r="G11" t="s">
+        <v>336</v>
+      </c>
+      <c r="H11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I11" t="s">
+        <v>361</v>
+      </c>
+      <c r="J11" t="s">
+        <v>362</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" t="s">
+        <v>363</v>
+      </c>
+      <c r="C12" t="s">
+        <v>364</v>
+      </c>
+      <c r="D12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" t="s">
+        <v>190</v>
+      </c>
+      <c r="I12" t="s">
+        <v>182</v>
+      </c>
+      <c r="J12" t="s">
+        <v>182</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>234</v>
+      </c>
+      <c r="B13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C13" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" t="s">
+        <v>236</v>
+      </c>
+      <c r="E13" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" t="s">
+        <v>204</v>
+      </c>
+      <c r="G13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" t="s">
+        <v>238</v>
+      </c>
+      <c r="J13" t="s">
+        <v>239</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" t="s">
+        <v>366</v>
+      </c>
+      <c r="D14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E14" t="s">
+        <v>226</v>
+      </c>
+      <c r="F14" t="s">
+        <v>204</v>
+      </c>
+      <c r="G14" t="s">
+        <v>241</v>
+      </c>
+      <c r="H14" t="s">
+        <v>367</v>
+      </c>
+      <c r="I14" t="s">
+        <v>243</v>
+      </c>
+      <c r="J14" t="s">
+        <v>244</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B15" t="s">
+        <v>368</v>
+      </c>
+      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" t="s">
+        <v>236</v>
+      </c>
+      <c r="E15" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G15" t="s">
+        <v>227</v>
+      </c>
+      <c r="H15" t="s">
+        <v>247</v>
+      </c>
+      <c r="I15" t="s">
+        <v>248</v>
+      </c>
+      <c r="J15" t="s">
+        <v>182</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" t="s">
+        <v>369</v>
+      </c>
+      <c r="C16" t="s">
+        <v>370</v>
+      </c>
+      <c r="D16" t="s">
+        <v>236</v>
+      </c>
+      <c r="E16" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" t="s">
+        <v>226</v>
+      </c>
+      <c r="G16" t="s">
+        <v>227</v>
+      </c>
+      <c r="H16" t="s">
+        <v>371</v>
+      </c>
+      <c r="I16" t="s">
+        <v>372</v>
+      </c>
+      <c r="J16" t="s">
+        <v>182</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" t="s">
+        <v>373</v>
+      </c>
+      <c r="C17" t="s">
+        <v>254</v>
+      </c>
+      <c r="D17" t="s">
+        <v>236</v>
+      </c>
+      <c r="E17" t="s">
+        <v>255</v>
+      </c>
+      <c r="F17" t="s">
+        <v>185</v>
+      </c>
+      <c r="G17" t="s">
+        <v>205</v>
+      </c>
+      <c r="H17" t="s">
+        <v>256</v>
+      </c>
+      <c r="I17" t="s">
+        <v>257</v>
+      </c>
+      <c r="J17" t="s">
+        <v>258</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B18" t="s">
+        <v>302</v>
+      </c>
+      <c r="C18" t="s">
+        <v>374</v>
+      </c>
+      <c r="D18" t="s">
+        <v>236</v>
+      </c>
+      <c r="E18" t="s">
+        <v>204</v>
+      </c>
+      <c r="F18" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18" t="s">
+        <v>227</v>
+      </c>
+      <c r="H18" t="s">
+        <v>375</v>
+      </c>
+      <c r="I18" t="s">
+        <v>261</v>
+      </c>
+      <c r="J18" t="s">
+        <v>182</v>
+      </c>
+      <c r="K18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19" t="s">
+        <v>376</v>
+      </c>
+      <c r="C19" t="s">
+        <v>377</v>
+      </c>
+      <c r="D19" t="s">
+        <v>236</v>
+      </c>
+      <c r="E19" t="s">
+        <v>226</v>
+      </c>
+      <c r="F19" t="s">
+        <v>204</v>
+      </c>
+      <c r="G19" t="s">
+        <v>241</v>
+      </c>
+      <c r="H19" t="s">
+        <v>378</v>
+      </c>
+      <c r="I19" t="s">
+        <v>265</v>
+      </c>
+      <c r="J19" t="s">
+        <v>182</v>
+      </c>
+      <c r="K19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>266</v>
+      </c>
+      <c r="B20" t="s">
+        <v>379</v>
+      </c>
+      <c r="C20" t="s">
+        <v>267</v>
+      </c>
+      <c r="D20" t="s">
+        <v>236</v>
+      </c>
+      <c r="E20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F20" t="s">
+        <v>204</v>
+      </c>
+      <c r="G20" t="s">
+        <v>227</v>
+      </c>
+      <c r="H20" t="s">
+        <v>380</v>
+      </c>
+      <c r="I20" t="s">
+        <v>269</v>
+      </c>
+      <c r="J20" t="s">
+        <v>182</v>
+      </c>
+      <c r="K20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" t="s">
+        <v>381</v>
+      </c>
+      <c r="C21" t="s">
+        <v>382</v>
+      </c>
+      <c r="D21" t="s">
+        <v>236</v>
+      </c>
+      <c r="E21" t="s">
+        <v>226</v>
+      </c>
+      <c r="F21" t="s">
+        <v>185</v>
+      </c>
+      <c r="G21" t="s">
+        <v>227</v>
+      </c>
+      <c r="H21" t="s">
+        <v>383</v>
+      </c>
+      <c r="I21" t="s">
+        <v>384</v>
+      </c>
+      <c r="J21" t="s">
+        <v>385</v>
+      </c>
+      <c r="K21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>275</v>
+      </c>
+      <c r="B22" t="s">
+        <v>386</v>
+      </c>
+      <c r="C22" t="s">
+        <v>387</v>
+      </c>
+      <c r="D22" t="s">
+        <v>277</v>
+      </c>
+      <c r="E22" t="s">
+        <v>177</v>
+      </c>
+      <c r="F22" t="s">
+        <v>177</v>
+      </c>
+      <c r="G22" t="s">
+        <v>278</v>
+      </c>
+      <c r="H22" t="s">
+        <v>388</v>
+      </c>
+      <c r="I22" t="s">
+        <v>182</v>
+      </c>
+      <c r="J22" t="s">
+        <v>280</v>
+      </c>
+      <c r="K22" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F493F04-F8C0-4690-8879-53ABE7C203D4}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F1" t="s">
+        <v>394</v>
+      </c>
+      <c r="G1" t="s">
+        <v>395</v>
+      </c>
+      <c r="H1" t="s">
+        <v>396</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E2" t="s">
+        <v>402</v>
+      </c>
+      <c r="F2" t="s">
+        <v>403</v>
+      </c>
+      <c r="G2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E3" t="s">
+        <v>402</v>
+      </c>
+      <c r="F3" t="s">
+        <v>398</v>
+      </c>
+      <c r="G3" t="s">
+        <v>404</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B4" t="s">
+        <v>399</v>
+      </c>
+      <c r="C4" t="s">
+        <v>409</v>
+      </c>
+      <c r="D4" t="s">
+        <v>410</v>
+      </c>
+      <c r="E4" t="s">
+        <v>402</v>
+      </c>
+      <c r="F4" t="s">
+        <v>398</v>
+      </c>
+      <c r="G4" t="s">
+        <v>404</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D5" t="s">
+        <v>413</v>
+      </c>
+      <c r="E5" t="s">
+        <v>402</v>
+      </c>
+      <c r="F5" t="s">
+        <v>398</v>
+      </c>
+      <c r="G5" t="s">
+        <v>404</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C6" t="s">
+        <v>415</v>
+      </c>
+      <c r="D6" t="s">
+        <v>416</v>
+      </c>
+      <c r="E6" t="s">
+        <v>402</v>
+      </c>
+      <c r="F6" t="s">
+        <v>398</v>
+      </c>
+      <c r="G6" t="s">
+        <v>404</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B7" t="s">
+        <v>399</v>
+      </c>
+      <c r="C7" t="s">
+        <v>418</v>
+      </c>
+      <c r="D7" t="s">
+        <v>419</v>
+      </c>
+      <c r="E7" t="s">
+        <v>402</v>
+      </c>
+      <c r="F7" t="s">
+        <v>398</v>
+      </c>
+      <c r="G7" t="s">
+        <v>404</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B8" t="s">
+        <v>421</v>
+      </c>
+      <c r="C8" t="s">
+        <v>422</v>
+      </c>
+      <c r="D8" t="s">
+        <v>423</v>
+      </c>
+      <c r="E8" t="s">
+        <v>402</v>
+      </c>
+      <c r="F8" t="s">
+        <v>403</v>
+      </c>
+      <c r="G8" t="s">
+        <v>404</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B9" t="s">
+        <v>421</v>
+      </c>
+      <c r="C9" t="s">
+        <v>425</v>
+      </c>
+      <c r="D9" t="s">
+        <v>426</v>
+      </c>
+      <c r="E9" t="s">
+        <v>402</v>
+      </c>
+      <c r="F9" t="s">
+        <v>420</v>
+      </c>
+      <c r="G9" t="s">
+        <v>404</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>427</v>
+      </c>
+      <c r="B10" t="s">
+        <v>421</v>
+      </c>
+      <c r="C10" t="s">
+        <v>428</v>
+      </c>
+      <c r="D10" t="s">
+        <v>426</v>
+      </c>
+      <c r="E10" t="s">
+        <v>402</v>
+      </c>
+      <c r="F10" t="s">
+        <v>420</v>
+      </c>
+      <c r="G10" t="s">
+        <v>404</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>429</v>
+      </c>
+      <c r="B11" t="s">
+        <v>421</v>
+      </c>
+      <c r="C11" t="s">
+        <v>430</v>
+      </c>
+      <c r="D11" t="s">
+        <v>431</v>
+      </c>
+      <c r="E11" t="s">
+        <v>402</v>
+      </c>
+      <c r="F11" t="s">
+        <v>403</v>
+      </c>
+      <c r="G11" t="s">
+        <v>404</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>432</v>
+      </c>
+      <c r="B12" t="s">
+        <v>433</v>
+      </c>
+      <c r="C12" t="s">
+        <v>434</v>
+      </c>
+      <c r="D12" t="s">
+        <v>435</v>
+      </c>
+      <c r="E12" t="s">
+        <v>402</v>
+      </c>
+      <c r="F12" t="s">
+        <v>403</v>
+      </c>
+      <c r="G12" t="s">
+        <v>404</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>436</v>
+      </c>
+      <c r="B13" t="s">
+        <v>433</v>
+      </c>
+      <c r="C13" t="s">
+        <v>437</v>
+      </c>
+      <c r="D13" t="s">
+        <v>438</v>
+      </c>
+      <c r="E13" t="s">
+        <v>402</v>
+      </c>
+      <c r="F13" t="s">
+        <v>432</v>
+      </c>
+      <c r="G13" s="5">
+        <v>45635</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>439</v>
+      </c>
+      <c r="B14" t="s">
+        <v>433</v>
+      </c>
+      <c r="C14" t="s">
+        <v>440</v>
+      </c>
+      <c r="D14" t="s">
+        <v>435</v>
+      </c>
+      <c r="E14" t="s">
+        <v>402</v>
+      </c>
+      <c r="F14" t="s">
+        <v>436</v>
+      </c>
+      <c r="G14" t="s">
+        <v>404</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>441</v>
+      </c>
+      <c r="B15" t="s">
+        <v>433</v>
+      </c>
+      <c r="C15" t="s">
+        <v>442</v>
+      </c>
+      <c r="D15" t="s">
+        <v>443</v>
+      </c>
+      <c r="E15" t="s">
+        <v>402</v>
+      </c>
+      <c r="F15" t="s">
+        <v>439</v>
+      </c>
+      <c r="G15" s="5">
+        <v>45642</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>444</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>445</v>
+      </c>
+      <c r="D16" t="s">
+        <v>446</v>
+      </c>
+      <c r="E16" t="s">
+        <v>402</v>
+      </c>
+      <c r="F16" t="s">
+        <v>403</v>
+      </c>
+      <c r="G16" t="s">
+        <v>404</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>447</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>448</v>
+      </c>
+      <c r="D17" t="s">
+        <v>449</v>
+      </c>
+      <c r="E17" t="s">
+        <v>402</v>
+      </c>
+      <c r="F17" t="s">
+        <v>444</v>
+      </c>
+      <c r="G17" t="s">
+        <v>404</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>450</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>451</v>
+      </c>
+      <c r="D18" t="s">
+        <v>452</v>
+      </c>
+      <c r="E18" t="s">
+        <v>402</v>
+      </c>
+      <c r="F18" t="s">
+        <v>444</v>
+      </c>
+      <c r="G18" t="s">
+        <v>404</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>453</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>454</v>
+      </c>
+      <c r="D19" t="s">
+        <v>455</v>
+      </c>
+      <c r="E19" t="s">
+        <v>402</v>
+      </c>
+      <c r="F19" t="s">
+        <v>403</v>
+      </c>
+      <c r="G19" t="s">
+        <v>404</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>456</v>
+      </c>
+      <c r="B20" t="s">
+        <v>457</v>
+      </c>
+      <c r="C20" t="s">
+        <v>458</v>
+      </c>
+      <c r="D20" t="s">
+        <v>459</v>
+      </c>
+      <c r="E20" t="s">
+        <v>402</v>
+      </c>
+      <c r="F20" t="s">
+        <v>453</v>
+      </c>
+      <c r="G20" t="s">
+        <v>404</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>460</v>
+      </c>
+      <c r="B21" t="s">
+        <v>457</v>
+      </c>
+      <c r="C21" t="s">
+        <v>461</v>
+      </c>
+      <c r="D21" t="s">
+        <v>462</v>
+      </c>
+      <c r="E21" t="s">
+        <v>402</v>
+      </c>
+      <c r="F21" t="s">
+        <v>436</v>
+      </c>
+      <c r="G21" t="s">
+        <v>404</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>463</v>
+      </c>
+      <c r="B22" t="s">
+        <v>457</v>
+      </c>
+      <c r="C22" t="s">
+        <v>464</v>
+      </c>
+      <c r="D22" t="s">
+        <v>465</v>
+      </c>
+      <c r="E22" t="s">
+        <v>402</v>
+      </c>
+      <c r="F22" t="s">
+        <v>436</v>
+      </c>
+      <c r="G22" t="s">
+        <v>404</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>466</v>
+      </c>
+      <c r="B23" t="s">
+        <v>467</v>
+      </c>
+      <c r="C23" t="s">
+        <v>468</v>
+      </c>
+      <c r="D23" t="s">
+        <v>469</v>
+      </c>
+      <c r="E23" t="s">
+        <v>402</v>
+      </c>
+      <c r="F23" t="s">
+        <v>403</v>
+      </c>
+      <c r="G23" t="s">
+        <v>404</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>470</v>
+      </c>
+      <c r="B24" t="s">
+        <v>467</v>
+      </c>
+      <c r="C24" t="s">
+        <v>471</v>
+      </c>
+      <c r="D24" t="s">
+        <v>469</v>
+      </c>
+      <c r="E24" t="s">
+        <v>402</v>
+      </c>
+      <c r="F24" t="s">
+        <v>403</v>
+      </c>
+      <c r="G24" t="s">
+        <v>404</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>472</v>
+      </c>
+      <c r="B25" t="s">
+        <v>467</v>
+      </c>
+      <c r="C25" t="s">
+        <v>473</v>
+      </c>
+      <c r="D25" t="s">
+        <v>474</v>
+      </c>
+      <c r="E25" t="s">
+        <v>402</v>
+      </c>
+      <c r="F25" t="s">
+        <v>403</v>
+      </c>
+      <c r="G25" t="s">
+        <v>404</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>475</v>
+      </c>
+      <c r="B26" t="s">
+        <v>476</v>
+      </c>
+      <c r="C26" t="s">
+        <v>477</v>
+      </c>
+      <c r="D26" t="s">
+        <v>478</v>
+      </c>
+      <c r="E26" t="s">
+        <v>402</v>
+      </c>
+      <c r="F26" t="s">
+        <v>403</v>
+      </c>
+      <c r="G26" t="s">
+        <v>404</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>81</v>
+      </c>
+      <c r="J26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>479</v>
+      </c>
+      <c r="B27" t="s">
+        <v>476</v>
+      </c>
+      <c r="C27" t="s">
+        <v>480</v>
+      </c>
+      <c r="D27" t="s">
+        <v>481</v>
+      </c>
+      <c r="E27" t="s">
+        <v>402</v>
+      </c>
+      <c r="F27" t="s">
+        <v>475</v>
+      </c>
+      <c r="G27" t="s">
+        <v>404</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>81</v>
+      </c>
+      <c r="J27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>482</v>
+      </c>
+      <c r="B28" t="s">
+        <v>476</v>
+      </c>
+      <c r="C28" t="s">
+        <v>483</v>
+      </c>
+      <c r="D28" t="s">
+        <v>484</v>
+      </c>
+      <c r="E28" t="s">
+        <v>402</v>
+      </c>
+      <c r="F28" t="s">
+        <v>475</v>
+      </c>
+      <c r="G28" t="s">
+        <v>404</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>